<commit_message>
delete venv & add downloads
</commit_message>
<xml_diff>
--- a/uploads/测试数据.xlsx
+++ b/uploads/测试数据.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD36148-20A1-406F-B07F-951A4A035686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="饼图" sheetId="1" r:id="rId1"/>
@@ -13,117 +12,409 @@
     <sheet name="柱状图" sheetId="3" r:id="rId3"/>
     <sheet name="仪表盘" sheetId="4" r:id="rId4"/>
     <sheet name="漏斗图" sheetId="5" r:id="rId5"/>
-    <sheet name="雷达图" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>吃饭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>打游戏</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>睡觉</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>时间占比</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>完成率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>展现</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>点击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>访问</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>咨询</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>订单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>销售</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>经理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>信息技术</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>客服</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>研发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>市场</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>预算分配</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>实际开销</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -131,24 +422,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -197,7 +774,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,26 +807,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,23 +842,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -469,21 +1012,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +1034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -499,7 +1042,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -508,28 +1051,29 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:B4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -537,7 +1081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -545,7 +1089,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -554,27 +1098,28 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -582,7 +1127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -590,7 +1135,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -599,22 +1144,23 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A81620-486D-4D5C-ABD0-CA813202B4FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -623,23 +1169,24 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C06BBF1-70B5-4368-9D96-49DB12572DB0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -647,7 +1194,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -655,7 +1202,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -663,7 +1210,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -671,7 +1218,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -680,117 +1227,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49FA269-1163-45C5-8FDA-AD9F6F855537}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>6500</v>
-      </c>
-      <c r="C2">
-        <v>4300</v>
-      </c>
-      <c r="D2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>16000</v>
-      </c>
-      <c r="C3">
-        <v>10000</v>
-      </c>
-      <c r="D3">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>30000</v>
-      </c>
-      <c r="C4">
-        <v>28000</v>
-      </c>
-      <c r="D4">
-        <v>28000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>38000</v>
-      </c>
-      <c r="C5">
-        <v>35000</v>
-      </c>
-      <c r="D5">
-        <v>31000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>52000</v>
-      </c>
-      <c r="C6">
-        <v>50000</v>
-      </c>
-      <c r="D6">
-        <v>42000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>25000</v>
-      </c>
-      <c r="C7">
-        <v>19000</v>
-      </c>
-      <c r="D7">
-        <v>21000</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>